<commit_message>
Modularity/Significance on yeast nets added and gene ontology dicts created
</commit_message>
<xml_diff>
--- a/Tables/Yeast_times.xlsx
+++ b/Tables/Yeast_times.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabio\Documents\Técnico\Tese Mestrado\Github\Tese\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FFFCEA-934A-4505-BB93-931D1746031B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E008E2EC-17ED-436C-8ADC-084C5D776C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Louvain</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Km</t>
+  </si>
+  <si>
+    <t>Cfinder</t>
   </si>
 </sst>
 </file>
@@ -323,8 +326,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F43EC0DD-C8FF-4A52-9B1D-83694B3F1412}" name="Tabela1" displayName="Tabela1" ref="B3:L13" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="B3:L13" xr:uid="{F43EC0DD-C8FF-4A52-9B1D-83694B3F1412}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F43EC0DD-C8FF-4A52-9B1D-83694B3F1412}" name="Tabela1" displayName="Tabela1" ref="B3:L14" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="B3:L14" xr:uid="{F43EC0DD-C8FF-4A52-9B1D-83694B3F1412}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{D7D785F4-95B3-42F0-9760-C0D5B32A505B}" name="Yeast networks" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{5DAFCF69-8083-4708-A2CC-39E21C33E780}" name="Sc" dataDxfId="9"/>
@@ -605,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:L13"/>
+  <dimension ref="B3:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,7 +808,7 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -818,6 +821,21 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>